<commit_message>
Final Back Up Commit
</commit_message>
<xml_diff>
--- a/Data/Input/COO_upload_Testcase1_231103_FAB.xlsx
+++ b/Data/Input/COO_upload_Testcase1_231103_FAB.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <x:si>
     <x:t>PO</x:t>
   </x:si>
@@ -86,10 +86,10 @@
     <x:t>Success</x:t>
   </x:si>
   <x:si>
-    <x:t>Test Updated</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12/26/2023 10:28:04</x:t>
+    <x:t>COO Updated + File Missing</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/26/2023 15:45:18</x:t>
   </x:si>
   <x:si>
     <x:t>13</x:t>
@@ -101,7 +101,7 @@
     <x:t>13325921_20231011T025110.pdf</x:t>
   </x:si>
   <x:si>
-    <x:t>12/26/2023 10:30:08</x:t>
+    <x:t>12/26/2023 15:47:25</x:t>
   </x:si>
   <x:si>
     <x:t>440399382</x:t>
@@ -116,142 +116,151 @@
     <x:t>Template Eur1_440547326.pdf</x:t>
   </x:si>
   <x:si>
+    <x:t>Failed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>No Records Found</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/26/2023 15:48:41</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>US|United States</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23000111.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/26/2023 15:50:48</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/26/2023 15:53:08</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IN|India</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INV253886.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FAILURE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UI Error</x:t>
+  </x:si>
+  <x:si>
+    <x:t>440407267</x:t>
+  </x:si>
+  <x:si>
+    <x:t>81</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IT|Italy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11649512_20220928T071246.pdf</x:t>
+  </x:si>
+  <x:si>
     <x:t>SUCCESS</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">COO Updated + File Uploaded </x:t>
   </x:si>
   <x:si>
-    <x:t>5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>US|United States</x:t>
-  </x:si>
-  <x:si>
-    <x:t>23000111.pdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FAILURE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Multiple Orders found</x:t>
+    <x:t>GB|United Kingdom</x:t>
+  </x:si>
+  <x:si>
+    <x:t>207</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HU|Hsdfcdfssdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Cannot find Country </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Korea, Republic of</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Wrong COO input format </x:t>
+  </x:si>
+  <x:si>
+    <x:t>257</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Missing key value: Order</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Missing key value : Line</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Missing key value : Shipment</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Missing key value : COO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>24</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25</x:t>
+  </x:si>
+  <x:si>
+    <x:t>26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27</x:t>
+  </x:si>
+  <x:si>
+    <x:t>28</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30</x:t>
+  </x:si>
+  <x:si>
+    <x:t>440572238</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>440571729</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>440571742</x:t>
+  </x:si>
+  <x:si>
+    <x:t>440096816</x:t>
+  </x:si>
+  <x:si>
+    <x:t>198</x:t>
+  </x:si>
+  <x:si>
+    <x:t>440sdasda554921</x:t>
+  </x:si>
+  <x:si>
+    <x:t>212</x:t>
   </x:si>
   <x:si>
     <x:t>Order not found</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IN|India</x:t>
-  </x:si>
-  <x:si>
-    <x:t>INV253886.pdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UI Error</x:t>
-  </x:si>
-  <x:si>
-    <x:t>440407267</x:t>
-  </x:si>
-  <x:si>
-    <x:t>81</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IT|Italy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11649512_20220928T071246.pdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>GB|United Kingdom</x:t>
-  </x:si>
-  <x:si>
-    <x:t>COO Updated + File Missing</x:t>
-  </x:si>
-  <x:si>
-    <x:t>207</x:t>
-  </x:si>
-  <x:si>
-    <x:t>HU|Hsdfcdfssdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Cannot find Country </x:t>
-  </x:si>
-  <x:si>
-    <x:t>Korea, Republic of</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">Wrong COO input format </x:t>
-  </x:si>
-  <x:si>
-    <x:t>257</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Missing key value: Order</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Missing key value : Line</x:t>
-  </x:si>
-  <x:si>
-    <x:t>21</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Missing key value : Shipment</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Missing key value : COO</x:t>
-  </x:si>
-  <x:si>
-    <x:t>23</x:t>
-  </x:si>
-  <x:si>
-    <x:t>24</x:t>
-  </x:si>
-  <x:si>
-    <x:t>25</x:t>
-  </x:si>
-  <x:si>
-    <x:t>26</x:t>
-  </x:si>
-  <x:si>
-    <x:t>27</x:t>
-  </x:si>
-  <x:si>
-    <x:t>28</x:t>
-  </x:si>
-  <x:si>
-    <x:t>29</x:t>
-  </x:si>
-  <x:si>
-    <x:t>30</x:t>
-  </x:si>
-  <x:si>
-    <x:t>440572238</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>440571729</x:t>
-  </x:si>
-  <x:si>
-    <x:t>10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>440571742</x:t>
-  </x:si>
-  <x:si>
-    <x:t>440096816</x:t>
-  </x:si>
-  <x:si>
-    <x:t>198</x:t>
-  </x:si>
-  <x:si>
-    <x:t>440sdasda554921</x:t>
-  </x:si>
-  <x:si>
-    <x:t>212</x:t>
   </x:si>
   <x:si>
     <x:t>440571932</x:t>
@@ -835,8 +844,8 @@
       <x:c r="H4" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="I4" s="1">
-        <x:v>45233.3736111111</x:v>
+      <x:c r="I4" s="1" t="s">
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:9">
@@ -847,25 +856,25 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="D5" s="0" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="G5" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="H5" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="I5" s="1" t="s">
         <x:v>31</x:v>
-      </x:c>
-      <x:c r="I5" s="1">
-        <x:v>45233.3736111111</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:9">
@@ -876,25 +885,25 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="D6" s="0" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="G6" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="H6" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="I6" s="1" t="s">
         <x:v>32</x:v>
-      </x:c>
-      <x:c r="I6" s="1">
-        <x:v>45233.3736111111</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:9">
@@ -917,10 +926,10 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="G7" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="H7" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="I7" s="1">
         <x:v>45233.3736111111</x:v>
@@ -928,28 +937,28 @@
     </x:row>
     <x:row r="8" spans="1:9">
       <x:c r="A8" s="7" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B8" s="0" t="n">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D8" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="G8" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H8" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="I8" s="1">
         <x:v>45233.3736111111</x:v>
@@ -957,25 +966,25 @@
     </x:row>
     <x:row r="9" spans="1:9">
       <x:c r="A9" s="7" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B9" s="0" t="n">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D9" s="0" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G9" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H9" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="I9" s="1">
         <x:v>45233.3736111111</x:v>
@@ -983,25 +992,25 @@
     </x:row>
     <x:row r="10" spans="1:9">
       <x:c r="A10" s="7" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B10" s="0" t="n">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="D10" s="0" t="n">
         <x:v>3</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="G10" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="H10" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="I10" s="1">
         <x:v>45233.3736111111</x:v>
@@ -1009,28 +1018,28 @@
     </x:row>
     <x:row r="11" spans="1:9">
       <x:c r="A11" s="7" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B11" s="0" t="n">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="D11" s="0" t="n">
         <x:v>4</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="F11" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="H11" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="I11" s="1">
         <x:v>45233.3736111111</x:v>
@@ -1042,7 +1051,7 @@
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D12" s="0" t="n">
         <x:v>5</x:v>
@@ -1054,10 +1063,10 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="H12" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="I12" s="1">
         <x:v>45233.3736111111</x:v>
@@ -1075,16 +1084,16 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="F13" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="H13" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="I13" s="1">
         <x:v>45233.3736111111</x:v>
@@ -1098,7 +1107,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="D14" s="13" t="s"/>
       <x:c r="E14" s="0" t="s">
@@ -1108,10 +1117,10 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="G14" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="H14" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="I14" s="1">
         <x:v>45233.3736111111</x:v>
@@ -1129,13 +1138,13 @@
       </x:c>
       <x:c r="E15" s="13" t="s"/>
       <x:c r="F15" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="G15" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="H15" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="I15" s="1">
         <x:v>45233.3736111111</x:v>
@@ -1149,19 +1158,19 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="D16" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="E16" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G16" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H16" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:9">
@@ -1172,7 +1181,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D17" s="0" t="n">
         <x:v>1</x:v>
@@ -1181,10 +1190,10 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="G17" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H17" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:9">
@@ -1195,7 +1204,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="D18" s="0" t="n">
         <x:v>1</x:v>
@@ -1204,10 +1213,10 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="G18" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H18" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:9">
@@ -1218,7 +1227,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="D19" s="0" t="n">
         <x:v>1</x:v>
@@ -1230,10 +1239,10 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="G19" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H19" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:9">
@@ -1244,22 +1253,22 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="D20" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="E20" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="F20" s="0" t="s">
         <x:v>35</x:v>
       </x:c>
       <x:c r="G20" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H20" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:9">
@@ -1270,7 +1279,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="D21" s="0" t="n">
         <x:v>1</x:v>
@@ -1282,10 +1291,10 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="G21" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H21" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:9">
@@ -1296,22 +1305,22 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="D22" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="E22" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F22" s="0" t="s">
         <x:v>35</x:v>
       </x:c>
       <x:c r="G22" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H22" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:9">
@@ -1322,33 +1331,33 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="D23" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="E23" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="F23" s="0" t="s">
         <x:v>35</x:v>
       </x:c>
       <x:c r="G23" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H23" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:9">
       <x:c r="A24" s="9" t="s">
-        <x:v>62</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="B24" s="10" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C24" s="10" t="s">
-        <x:v>63</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="E24" s="0" t="s">
         <x:v>12</x:v>
@@ -1357,21 +1366,21 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="G24" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H24" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:9">
       <x:c r="A25" s="9" t="s">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="B25" s="10" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C25" s="10" t="s">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="E25" s="0" t="s">
         <x:v>18</x:v>
@@ -1380,21 +1389,21 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="G25" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H25" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:9">
       <x:c r="A26" s="9" t="s">
-        <x:v>66</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="B26" s="10" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C26" s="10" t="s">
-        <x:v>63</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="E26" s="0" t="s">
         <x:v>23</x:v>
@@ -1403,67 +1412,67 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="G26" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H26" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:9">
       <x:c r="A27" s="9" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B27" s="10" t="n">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C27" s="10" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="E27" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="F27" s="0" t="s">
         <x:v>35</x:v>
       </x:c>
       <x:c r="G27" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H27" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:9">
       <x:c r="A28" s="9" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B28" s="10" t="n">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C28" s="10" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="E28" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="F28" s="0" t="s">
         <x:v>35</x:v>
       </x:c>
       <x:c r="G28" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H28" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:9">
       <x:c r="A29" s="9" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B29" s="10" t="n">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C29" s="10" t="s">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="E29" s="0" t="s">
         <x:v>34</x:v>
@@ -1472,87 +1481,87 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="G29" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H29" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:9">
       <x:c r="A30" s="9" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B30" s="10" t="n">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C30" s="10" t="s">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="E30" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F30" s="0" t="s">
         <x:v>35</x:v>
       </x:c>
       <x:c r="G30" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H30" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:9">
       <x:c r="A31" s="9" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B31" s="10" t="n">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C31" s="10" t="s">
-        <x:v>48</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="E31" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G31" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H31" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>15</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:9">
       <x:c r="A32" s="9" t="s">
-        <x:v>67</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="B32" s="10" t="n">
         <x:v>1359</x:v>
       </x:c>
       <x:c r="C32" s="10" t="s">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="E32" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F32" s="0" t="s">
         <x:v>24</x:v>
       </x:c>
       <x:c r="G32" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="H32" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:9">
       <x:c r="A33" s="9" t="s">
-        <x:v>69</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="B33" s="10" t="n">
         <x:v>66</x:v>
       </x:c>
       <x:c r="C33" s="10" t="s">
-        <x:v>70</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="E33" s="0" t="s">
         <x:v>18</x:v>
@@ -1561,21 +1570,21 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="G33" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="H33" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>73</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:9">
       <x:c r="A34" s="9" t="s">
-        <x:v>71</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="B34" s="10" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C34" s="10" t="s">
-        <x:v>72</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E34" s="0" t="s">
         <x:v>18</x:v>
@@ -1584,21 +1593,21 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="G34" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H34" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:9">
       <x:c r="A35" s="9" t="s">
-        <x:v>71</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="B35" s="10" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C35" s="10" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E35" s="0" t="s">
         <x:v>18</x:v>
@@ -1607,21 +1616,21 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="G35" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H35" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:9">
       <x:c r="A36" s="9" t="s">
-        <x:v>71</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="B36" s="10" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C36" s="10" t="s">
-        <x:v>63</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="E36" s="0" t="s">
         <x:v>18</x:v>
@@ -1630,21 +1639,21 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="G36" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H36" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:9">
       <x:c r="A37" s="9" t="s">
-        <x:v>71</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="B37" s="10" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C37" s="10" t="s">
-        <x:v>73</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="E37" s="0" t="s">
         <x:v>18</x:v>
@@ -1653,15 +1662,15 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="G37" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H37" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:9">
       <x:c r="A38" s="9" t="s">
-        <x:v>71</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="B38" s="10" t="s">
         <x:v>10</x:v>
@@ -1676,19 +1685,19 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="G38" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H38" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:9">
       <x:c r="A39" s="9" t="s">
-        <x:v>74</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B39" s="5" t="s"/>
       <x:c r="C39" s="10" t="s">
-        <x:v>75</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="E39" s="0" t="s">
         <x:v>18</x:v>
@@ -1697,19 +1706,19 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="G39" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H39" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:9">
       <x:c r="A40" s="9" t="s">
-        <x:v>74</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B40" s="5" t="s"/>
       <x:c r="C40" s="10" t="s">
-        <x:v>76</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="E40" s="0" t="s">
         <x:v>18</x:v>
@@ -1718,19 +1727,19 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="G40" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H40" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:9">
       <x:c r="A41" s="9" t="s">
-        <x:v>74</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B41" s="5" t="s"/>
       <x:c r="C41" s="10" t="s">
-        <x:v>77</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="E41" s="0" t="s">
         <x:v>18</x:v>
@@ -1739,19 +1748,19 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="G41" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H41" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:9">
       <x:c r="A42" s="9" t="s">
-        <x:v>78</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B42" s="5" t="s"/>
       <x:c r="C42" s="10" t="s">
-        <x:v>72</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E42" s="0" t="s">
         <x:v>18</x:v>
@@ -1760,19 +1769,19 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="G42" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H42" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:9">
       <x:c r="A43" s="9" t="s">
-        <x:v>78</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B43" s="5" t="s"/>
       <x:c r="C43" s="10" t="s">
-        <x:v>63</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="E43" s="0" t="s">
         <x:v>18</x:v>
@@ -1781,19 +1790,19 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="G43" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H43" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:9">
       <x:c r="A44" s="9" t="s">
-        <x:v>78</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B44" s="5" t="s"/>
       <x:c r="C44" s="10" t="s">
-        <x:v>73</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="E44" s="0" t="s">
         <x:v>18</x:v>
@@ -1802,10 +1811,10 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="G44" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="H44" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>43</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
End to End Commit
</commit_message>
<xml_diff>
--- a/Data/Input/COO_upload_Testcase1_231103_FAB.xlsx
+++ b/Data/Input/COO_upload_Testcase1_231103_FAB.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <x:si>
     <x:t>PO</x:t>
   </x:si>
@@ -83,99 +83,90 @@
     <x:t>13313488_20231009T050659.pdf</x:t>
   </x:si>
   <x:si>
-    <x:t>Success</x:t>
+    <x:t>Failed</x:t>
+  </x:si>
+  <x:si>
+    <x:t>System error.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/27/2023 11:26:05</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>KR|Korea, Republic of</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13325921_20231011T025110.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SUCCESS</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">COO Updated + File Uploaded </x:t>
+  </x:si>
+  <x:si>
+    <x:t>440399382</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CN|China</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Template Eur1_440547326.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>US|United States</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23000111.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>FAILURE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Multiple Orders found</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Order not found</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IN|India</x:t>
+  </x:si>
+  <x:si>
+    <x:t>INV253886.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>UI Error</x:t>
+  </x:si>
+  <x:si>
+    <x:t>440407267</x:t>
+  </x:si>
+  <x:si>
+    <x:t>81</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IT|Italy</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11649512_20220928T071246.pdf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>GB|United Kingdom</x:t>
   </x:si>
   <x:si>
     <x:t>COO Updated + File Missing</x:t>
   </x:si>
   <x:si>
-    <x:t>12/26/2023 15:45:18</x:t>
-  </x:si>
-  <x:si>
-    <x:t>13</x:t>
-  </x:si>
-  <x:si>
-    <x:t>KR|Korea, Republic of</x:t>
-  </x:si>
-  <x:si>
-    <x:t>13325921_20231011T025110.pdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12/26/2023 15:47:25</x:t>
-  </x:si>
-  <x:si>
-    <x:t>440399382</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>CN|China</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Template Eur1_440547326.pdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Failed</x:t>
-  </x:si>
-  <x:si>
-    <x:t>No Records Found</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12/26/2023 15:48:41</x:t>
-  </x:si>
-  <x:si>
-    <x:t>5</x:t>
-  </x:si>
-  <x:si>
-    <x:t>US|United States</x:t>
-  </x:si>
-  <x:si>
-    <x:t>23000111.pdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12/26/2023 15:50:48</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12/26/2023 15:53:08</x:t>
-  </x:si>
-  <x:si>
-    <x:t>8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IN|India</x:t>
-  </x:si>
-  <x:si>
-    <x:t>INV253886.pdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>FAILURE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>UI Error</x:t>
-  </x:si>
-  <x:si>
-    <x:t>440407267</x:t>
-  </x:si>
-  <x:si>
-    <x:t>81</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IT|Italy</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11649512_20220928T071246.pdf</x:t>
-  </x:si>
-  <x:si>
-    <x:t>SUCCESS</x:t>
-  </x:si>
-  <x:si>
-    <x:t xml:space="preserve">COO Updated + File Uploaded </x:t>
-  </x:si>
-  <x:si>
-    <x:t>GB|United Kingdom</x:t>
-  </x:si>
-  <x:si>
     <x:t>207</x:t>
   </x:si>
   <x:si>
@@ -258,9 +249,6 @@
   </x:si>
   <x:si>
     <x:t>212</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Order not found</x:t>
   </x:si>
   <x:si>
     <x:t>440571932</x:t>
@@ -810,42 +798,42 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="G3" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H3" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="I3" s="1" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="I3" s="1">
+        <x:v>45233.3736111111</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:9">
       <x:c r="A4" s="7" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B4" s="0" t="n">
         <x:v>38</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="D4" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G4" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H4" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="I4" s="1" t="s">
-        <x:v>27</x:v>
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="I4" s="1">
+        <x:v>45233.3736111111</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:9">
@@ -856,80 +844,80 @@
         <x:v>38</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D5" s="0" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="G5" s="0" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="F5" s="0" t="s">
+      <x:c r="H5" s="0" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="G5" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="H5" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="I5" s="1" t="s">
-        <x:v>31</x:v>
+      <x:c r="I5" s="1">
+        <x:v>45233.3736111111</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:9">
       <x:c r="A6" s="7" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B6" s="0" t="n">
         <x:v>38</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D6" s="0" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="F6" s="0" t="s">
-        <x:v>30</x:v>
-      </x:c>
-      <x:c r="G6" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
       <x:c r="H6" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="I6" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="I6" s="1">
+        <x:v>45233.3736111111</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:9">
       <x:c r="A7" s="7" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B7" s="0" t="n">
         <x:v>38</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="D7" s="0" t="n">
         <x:v>3</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="F7" s="0" t="s">
+      <x:c r="G7" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="H7" s="0" t="s">
         <x:v>35</x:v>
-      </x:c>
-      <x:c r="G7" s="0" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="H7" s="0" t="s">
-        <x:v>37</x:v>
       </x:c>
       <x:c r="I7" s="1">
         <x:v>45233.3736111111</x:v>
@@ -937,28 +925,28 @@
     </x:row>
     <x:row r="8" spans="1:9">
       <x:c r="A8" s="7" t="s">
-        <x:v>38</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B8" s="0" t="n">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="D8" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="G8" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H8" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="I8" s="1">
         <x:v>45233.3736111111</x:v>
@@ -966,25 +954,25 @@
     </x:row>
     <x:row r="9" spans="1:9">
       <x:c r="A9" s="7" t="s">
-        <x:v>38</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B9" s="0" t="n">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="D9" s="0" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="G9" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H9" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="I9" s="1">
         <x:v>45233.3736111111</x:v>
@@ -992,25 +980,25 @@
     </x:row>
     <x:row r="10" spans="1:9">
       <x:c r="A10" s="7" t="s">
-        <x:v>38</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B10" s="0" t="n">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="D10" s="0" t="n">
         <x:v>3</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="G10" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="H10" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="I10" s="1">
         <x:v>45233.3736111111</x:v>
@@ -1018,28 +1006,28 @@
     </x:row>
     <x:row r="11" spans="1:9">
       <x:c r="A11" s="7" t="s">
-        <x:v>38</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B11" s="0" t="n">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="D11" s="0" t="n">
         <x:v>4</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="F11" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="H11" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="I11" s="1">
         <x:v>45233.3736111111</x:v>
@@ -1051,22 +1039,22 @@
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="D12" s="0" t="n">
         <x:v>5</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F12" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="H12" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="I12" s="1">
         <x:v>45233.3736111111</x:v>
@@ -1084,16 +1072,16 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F13" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="H13" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="I13" s="1">
         <x:v>45233.3736111111</x:v>
@@ -1107,20 +1095,20 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D14" s="13" t="s"/>
       <x:c r="E14" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="F14" s="0" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="F14" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
       <x:c r="G14" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="H14" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="I14" s="1">
         <x:v>45233.3736111111</x:v>
@@ -1138,13 +1126,13 @@
       </x:c>
       <x:c r="E15" s="13" t="s"/>
       <x:c r="F15" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="G15" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="H15" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="I15" s="1">
         <x:v>45233.3736111111</x:v>
@@ -1158,19 +1146,19 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="D16" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="E16" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="G16" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H16" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:9">
@@ -1181,7 +1169,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="D17" s="0" t="n">
         <x:v>1</x:v>
@@ -1190,10 +1178,10 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="G17" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H17" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:9">
@@ -1204,7 +1192,7 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="D18" s="0" t="n">
         <x:v>1</x:v>
@@ -1213,10 +1201,10 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="G18" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H18" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:9">
@@ -1227,22 +1215,22 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="D19" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="E19" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F19" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G19" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H19" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:9">
@@ -1253,22 +1241,22 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D20" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="E20" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F20" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G20" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H20" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:9">
@@ -1279,22 +1267,22 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="D21" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="E21" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="F21" s="0" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="F21" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
       <x:c r="G21" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H21" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:9">
@@ -1305,22 +1293,22 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C22" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="D22" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="E22" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="F22" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G22" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H22" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="23" spans="1:9">
@@ -1331,490 +1319,490 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="D23" s="0" t="n">
         <x:v>1</x:v>
       </x:c>
       <x:c r="E23" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F23" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G23" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H23" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:9">
       <x:c r="A24" s="9" t="s">
-        <x:v>64</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="B24" s="10" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C24" s="10" t="s">
-        <x:v>65</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="E24" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="F24" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G24" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H24" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:9">
       <x:c r="A25" s="9" t="s">
-        <x:v>66</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="B25" s="10" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C25" s="10" t="s">
-        <x:v>67</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="E25" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="F25" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G25" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H25" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:9">
       <x:c r="A26" s="9" t="s">
-        <x:v>68</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="B26" s="10" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C26" s="10" t="s">
-        <x:v>65</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="E26" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F26" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G26" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H26" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="27" spans="1:9">
       <x:c r="A27" s="9" t="s">
-        <x:v>38</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B27" s="10" t="n">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C27" s="10" t="s">
-        <x:v>39</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E27" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F27" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G27" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H27" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="1:9">
       <x:c r="A28" s="9" t="s">
-        <x:v>38</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B28" s="10" t="n">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C28" s="10" t="s">
-        <x:v>39</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E28" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="F28" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G28" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H28" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="29" spans="1:9">
       <x:c r="A29" s="9" t="s">
-        <x:v>38</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B29" s="10" t="n">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C29" s="10" t="s">
-        <x:v>45</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="E29" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="F29" s="0" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="F29" s="0" t="s">
-        <x:v>35</x:v>
-      </x:c>
       <x:c r="G29" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H29" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="30" spans="1:9">
       <x:c r="A30" s="9" t="s">
-        <x:v>38</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B30" s="10" t="n">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C30" s="10" t="s">
-        <x:v>45</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="E30" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="F30" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="G30" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H30" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:9">
       <x:c r="A31" s="9" t="s">
-        <x:v>38</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="B31" s="10" t="n">
         <x:v>1001</x:v>
       </x:c>
       <x:c r="C31" s="10" t="s">
-        <x:v>50</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="E31" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="G31" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H31" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>41</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:9">
       <x:c r="A32" s="9" t="s">
-        <x:v>69</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="B32" s="10" t="n">
         <x:v>1359</x:v>
       </x:c>
       <x:c r="C32" s="10" t="s">
-        <x:v>70</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="E32" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F32" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G32" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="H32" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>44</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:9">
       <x:c r="A33" s="9" t="s">
-        <x:v>71</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="B33" s="10" t="n">
         <x:v>66</x:v>
       </x:c>
       <x:c r="C33" s="10" t="s">
-        <x:v>72</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="E33" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="F33" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G33" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="H33" s="0" t="s">
-        <x:v>73</x:v>
+        <x:v>31</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:9">
       <x:c r="A34" s="9" t="s">
-        <x:v>74</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="B34" s="10" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C34" s="10" t="s">
-        <x:v>75</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="E34" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="F34" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G34" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H34" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:9">
       <x:c r="A35" s="9" t="s">
-        <x:v>74</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="B35" s="10" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C35" s="10" t="s">
-        <x:v>28</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="E35" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="F35" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G35" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H35" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:9">
       <x:c r="A36" s="9" t="s">
-        <x:v>74</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="B36" s="10" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C36" s="10" t="s">
-        <x:v>65</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="E36" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="F36" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G36" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H36" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:9">
       <x:c r="A37" s="9" t="s">
-        <x:v>74</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="B37" s="10" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C37" s="10" t="s">
-        <x:v>76</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="E37" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="F37" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G37" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H37" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:9">
       <x:c r="A38" s="9" t="s">
-        <x:v>74</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="B38" s="10" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="C38" s="10" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="E38" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="F38" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G38" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H38" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:9">
       <x:c r="A39" s="9" t="s">
-        <x:v>77</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="B39" s="5" t="s"/>
       <x:c r="C39" s="10" t="s">
-        <x:v>78</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="E39" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="F39" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G39" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H39" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:9">
       <x:c r="A40" s="9" t="s">
-        <x:v>77</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="B40" s="5" t="s"/>
       <x:c r="C40" s="10" t="s">
-        <x:v>79</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="E40" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="F40" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G40" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H40" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:9">
       <x:c r="A41" s="9" t="s">
-        <x:v>77</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="B41" s="5" t="s"/>
       <x:c r="C41" s="10" t="s">
-        <x:v>80</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="E41" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="F41" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G41" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H41" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:9">
       <x:c r="A42" s="9" t="s">
-        <x:v>81</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B42" s="5" t="s"/>
       <x:c r="C42" s="10" t="s">
-        <x:v>75</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="E42" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="F42" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G42" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H42" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:9">
       <x:c r="A43" s="9" t="s">
-        <x:v>81</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B43" s="5" t="s"/>
       <x:c r="C43" s="10" t="s">
-        <x:v>65</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="E43" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="F43" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G43" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H43" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:9">
       <x:c r="A44" s="9" t="s">
-        <x:v>81</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="B44" s="5" t="s"/>
       <x:c r="C44" s="10" t="s">
-        <x:v>76</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="E44" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
       <x:c r="F44" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G44" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="H44" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>21</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>